<commit_message>
done DZ3 for Economics
</commit_message>
<xml_diff>
--- a/Экономика часть 2/ДЗ3/Лист Microsoft Excel.xlsx
+++ b/Экономика часть 2/ДЗ3/Лист Microsoft Excel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Учёба\8 Семестр\Экономика часть 2\ДЗ2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Учёба\8 Семестр\Экономика часть 2\ДЗ3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBD798-04E5-45FF-9DED-67112DDE4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEECCD29-002D-42D7-8B08-262D2B4C958A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="322">
   <si>
     <t xml:space="preserve">Наименование показателя </t>
   </si>
@@ -1034,19 +1036,1035 @@
   <si>
     <t>CFO =</t>
   </si>
+  <si>
+    <t>Материальные затраты</t>
+  </si>
+  <si>
+    <t>Расходы на оплату труда</t>
+  </si>
+  <si>
+    <t>Отчисления на социальные нужды</t>
+  </si>
+  <si>
+    <t>Амортизация</t>
+  </si>
+  <si>
+    <t>Прочие производственные затраты</t>
+  </si>
+  <si>
+    <t>Итого по элементам</t>
+  </si>
+  <si>
+    <t>Вид затрат</t>
+  </si>
+  <si>
+    <r>
+      <t>Шифр</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Наименование</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Источник или формула</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>МЗ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Материальные затраты</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ЗП</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Заработная плата</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5620+5630</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>АМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Амортизация</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ПЗ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Прочие затраты</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>З</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Затраты</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>МЗ%</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>МЗ% = МЗ / З * 100</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ЗП%</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ЗП% = ЗП / З * 100</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>АМ%</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>АМ% = АМ / З * 100</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ПЗ%</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ПЗ% = ПЗ / З * 100</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>МЗ-ЕМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Материалоемкость</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>МЗ-ЕМ = МЗ / В</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ЗП-ЕМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Зарплатоемкость</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ЗП-ЕМ = ЗП / В</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>АМ-ЕМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Амортизациоемкость</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>АМ-ЕМ = АМ / В</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ПЗ-ЕМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Емкость прочих затрат</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ПЗ-ЕМ = ПЗ / В</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>З-ЕМ</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Затратоемкость</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>З-ЕМ = З / В</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>КР</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Коммерческие расходы</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>УР</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Управленческие расходы</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Показатель</t>
+  </si>
+  <si>
+    <r>
+      <t>PC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TC</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>OP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>ЗАП</t>
+  </si>
+  <si>
+    <t>Запасы</t>
+  </si>
+  <si>
+    <t>ОА</t>
+  </si>
+  <si>
+    <t>Оборотные активы</t>
+  </si>
+  <si>
+    <t>А</t>
+  </si>
+  <si>
+    <t>Активы</t>
+  </si>
+  <si>
+    <t>ОБ-А</t>
+  </si>
+  <si>
+    <t>Оборачиваемость активов</t>
+  </si>
+  <si>
+    <t>ОБ-А = В / А</t>
+  </si>
+  <si>
+    <t>ОБ-ОА</t>
+  </si>
+  <si>
+    <t>Оборачиваемость оборотных активов</t>
+  </si>
+  <si>
+    <t>ОБ-ОА = В / ОА</t>
+  </si>
+  <si>
+    <t>ОБ-</t>
+  </si>
+  <si>
+    <t>Оборачиваемость запасов</t>
+  </si>
+  <si>
+    <t>ОБ-ЗАП = В / ЗАП</t>
+  </si>
+  <si>
+    <t>ДЕБ</t>
+  </si>
+  <si>
+    <t>Дебиторская задолженность</t>
+  </si>
+  <si>
+    <t>КРЕД</t>
+  </si>
+  <si>
+    <t>Кредиторская задолженность</t>
+  </si>
+  <si>
+    <t>Т</t>
+  </si>
+  <si>
+    <t>Длительность года</t>
+  </si>
+  <si>
+    <t>360 дней</t>
+  </si>
+  <si>
+    <t>Д-ЗАП</t>
+  </si>
+  <si>
+    <t>Длительность оборота запасов</t>
+  </si>
+  <si>
+    <t>Д-ЗАП = Т * ЗАП / В</t>
+  </si>
+  <si>
+    <t>Д-ДЕБ</t>
+  </si>
+  <si>
+    <t>Длительность оборота дебиторской задолженности</t>
+  </si>
+  <si>
+    <t>Д-ДЕБ = Т * ДЕБ / В</t>
+  </si>
+  <si>
+    <t>Д-КРЕД</t>
+  </si>
+  <si>
+    <t>Длительность оборота кредиторской задолженности</t>
+  </si>
+  <si>
+    <t>Д-КРЕД = Т * КРЕД / В</t>
+  </si>
+  <si>
+    <t>Ц-ОПЕР</t>
+  </si>
+  <si>
+    <t>Операционный цикл</t>
+  </si>
+  <si>
+    <t>Ц-ОПЕР = Д-ЗАП + Д-ДЕБ</t>
+  </si>
+  <si>
+    <t>Ц-ФИН</t>
+  </si>
+  <si>
+    <t>Финансовый цикл</t>
+  </si>
+  <si>
+    <t>Ц-ФИН = Ц-ОПЕР - Д-КРЕД</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROS </t>
+  </si>
+  <si>
+    <r>
+      <t>Рентабельность продаж (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Return On Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ROS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> = П-ЧИСТ / В</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ROA </t>
+  </si>
+  <si>
+    <r>
+      <t>Рентабельность активов (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Return On Assets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ROA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> = П-ЧИСТ / А</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ROE </t>
+  </si>
+  <si>
+    <r>
+      <t>Рентабельность собственного капитала (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Return On Equity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ROE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> = П-ЧИСТ / СК</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ROI </t>
+  </si>
+  <si>
+    <r>
+      <t>Рентабельность инвестиционного капитала (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Return On Investment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t>s)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ROI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> = П-ЧИСТ / ИК</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="\(_-* #,##0_-\);\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="0.000%"/>
+    <numFmt numFmtId="172" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1099,6 +2117,23 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1108,7 +2143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1223,12 +2258,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1362,41 +2408,17 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1411,6 +2433,88 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5910,32 +7014,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:S189"/>
+  <dimension ref="A1:S265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J118" sqref="J118"/>
+    <sheetView tabSelected="1" topLeftCell="A257" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E274" sqref="E274"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="66" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="74.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
-    <col min="16" max="16" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -5952,7 +7058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -5963,7 +7069,7 @@
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
-    <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -5974,7 +7080,7 @@
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -5991,7 +7097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
@@ -6008,7 +7114,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
@@ -6025,7 +7131,7 @@
         <v>459427</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
@@ -6042,7 +7148,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -6059,7 +7165,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -6076,7 +7182,7 @@
         <v>31934</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>71</v>
       </c>
@@ -6093,7 +7199,7 @@
         <v>13746</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
         <v>12</v>
       </c>
@@ -6122,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
@@ -6133,7 +7239,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -6150,7 +7256,7 @@
         <v>43900</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="5" t="s">
         <v>15</v>
       </c>
@@ -6167,7 +7273,7 @@
         <v>3397</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="5" t="s">
         <v>16</v>
       </c>
@@ -6184,7 +7290,7 @@
         <v>205421</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="5" t="s">
         <v>17</v>
       </c>
@@ -6201,7 +7307,7 @@
         <v>128000</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="5" t="s">
         <v>18</v>
       </c>
@@ -6218,7 +7324,7 @@
         <v>7113</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
@@ -6247,7 +7353,7 @@
         <v>13428</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
@@ -6276,7 +7382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
         <v>21</v>
       </c>
@@ -6287,7 +7393,7 @@
       <c r="E21" s="11"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
         <v>22</v>
       </c>
@@ -6298,7 +7404,7 @@
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
     </row>
-    <row r="23" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -6315,7 +7421,7 @@
         <v>334345</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="5" t="s">
         <v>24</v>
       </c>
@@ -6332,7 +7438,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>25</v>
       </c>
@@ -6349,7 +7455,7 @@
         <v>511720</v>
       </c>
     </row>
-    <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="5" t="s">
         <v>26</v>
       </c>
@@ -6366,7 +7472,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
@@ -6383,7 +7489,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -6400,7 +7506,7 @@
         <v>243087</v>
       </c>
     </row>
-    <row r="29" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
@@ -6429,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="3" t="s">
         <v>30</v>
       </c>
@@ -6440,7 +7546,7 @@
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
     </row>
-    <row r="31" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="5" t="s">
         <v>31</v>
       </c>
@@ -6457,7 +7563,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="5" t="s">
         <v>32</v>
       </c>
@@ -6474,7 +7580,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="5" t="s">
         <v>33</v>
       </c>
@@ -6491,7 +7597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="3" t="s">
         <v>34</v>
       </c>
@@ -6520,7 +7626,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="3" t="s">
         <v>35</v>
       </c>
@@ -6531,7 +7637,7 @@
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
     </row>
-    <row r="36" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="5" t="s">
         <v>36</v>
       </c>
@@ -6548,7 +7654,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="37" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" s="5" t="s">
         <v>37</v>
       </c>
@@ -6565,7 +7671,7 @@
         <v>208644</v>
       </c>
     </row>
-    <row r="38" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="5" t="s">
         <v>38</v>
       </c>
@@ -6582,7 +7688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="5" t="s">
         <v>39</v>
       </c>
@@ -6599,7 +7705,7 @@
         <v>91855</v>
       </c>
     </row>
-    <row r="40" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="3" t="s">
         <v>40</v>
       </c>
@@ -6628,7 +7734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="3" t="s">
         <v>20</v>
       </c>
@@ -6657,8 +7763,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H46" s="7" t="s">
         <v>41</v>
       </c>
@@ -6678,7 +7784,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H47" s="8" t="s">
         <v>44</v>
       </c>
@@ -6701,7 +7807,7 @@
         <v>906366</v>
       </c>
     </row>
-    <row r="48" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H48" s="8" t="s">
         <v>47</v>
       </c>
@@ -6724,7 +7830,7 @@
         <v>505107</v>
       </c>
     </row>
-    <row r="49" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H49" s="8" t="s">
         <v>49</v>
       </c>
@@ -6747,7 +7853,7 @@
         <v>401259</v>
       </c>
     </row>
-    <row r="50" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H50" s="10" t="s">
         <v>51</v>
       </c>
@@ -6770,7 +7876,7 @@
         <v>0.55728811539709122</v>
       </c>
     </row>
-    <row r="51" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H51" s="10" t="s">
         <v>53</v>
       </c>
@@ -6793,7 +7899,7 @@
         <v>0.44271188460290878</v>
       </c>
     </row>
-    <row r="52" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H52" s="8" t="s">
         <v>55</v>
       </c>
@@ -6816,7 +7922,7 @@
         <v>0.79440395797326113</v>
       </c>
     </row>
-    <row r="53" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H53" s="8" t="s">
         <v>58</v>
       </c>
@@ -6839,7 +7945,7 @@
         <v>605021</v>
       </c>
     </row>
-    <row r="54" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H54" s="8" t="s">
         <v>60</v>
       </c>
@@ -6862,7 +7968,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="55" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H55" s="8" t="s">
         <v>62</v>
       </c>
@@ -6885,7 +7991,7 @@
         <v>300499</v>
       </c>
     </row>
-    <row r="56" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H56" s="10" t="s">
         <v>64</v>
       </c>
@@ -6908,7 +8014,7 @@
         <v>0.6675239362465053</v>
       </c>
     </row>
-    <row r="57" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H57" s="10" t="s">
         <v>66</v>
       </c>
@@ -6931,7 +8037,7 @@
         <v>9.3339776646520281E-4</v>
       </c>
     </row>
-    <row r="58" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H58" s="10" t="s">
         <v>68</v>
       </c>
@@ -6954,13 +8060,13 @@
         <v>0.33154266598702953</v>
       </c>
     </row>
-    <row r="59" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:13" x14ac:dyDescent="0.3">
       <c r="K59" s="18"/>
       <c r="L59" s="18"/>
       <c r="M59" s="18"/>
     </row>
-    <row r="73" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="8:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P74" s="1" t="s">
         <v>72</v>
       </c>
@@ -6974,7 +8080,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H75" s="20" t="s">
         <v>78</v>
       </c>
@@ -7006,7 +8112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="76" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H76" s="23" t="s">
         <v>81</v>
       </c>
@@ -7041,7 +8147,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="77" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H77" s="23" t="s">
         <v>84</v>
       </c>
@@ -7079,25 +8185,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H78" s="59" t="s">
+    <row r="78" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H78" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="I78" s="61" t="s">
+      <c r="I78" s="53" t="s">
         <v>88</v>
       </c>
       <c r="J78" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="K78" s="63">
+      <c r="K78" s="55">
         <f>D7+D14</f>
         <v>689248</v>
       </c>
-      <c r="L78" s="63">
+      <c r="L78" s="55">
         <f t="shared" ref="L78:M78" si="2">E7+E14</f>
         <v>521696</v>
       </c>
-      <c r="M78" s="63">
+      <c r="M78" s="55">
         <f t="shared" si="2"/>
         <v>503327</v>
       </c>
@@ -7117,15 +8223,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H79" s="60"/>
-      <c r="I79" s="62"/>
+    <row r="79" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H79" s="52"/>
+      <c r="I79" s="54"/>
       <c r="J79" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="K79" s="60"/>
-      <c r="L79" s="60"/>
-      <c r="M79" s="60"/>
+      <c r="K79" s="52"/>
+      <c r="L79" s="52"/>
+      <c r="M79" s="52"/>
       <c r="P79" s="5" t="s">
         <v>77</v>
       </c>
@@ -7142,7 +8248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="8:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="8:19" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H80" s="23" t="s">
         <v>91</v>
       </c>
@@ -7165,7 +8271,7 @@
         <v>0.55532422884353561</v>
       </c>
     </row>
-    <row r="81" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H81" s="23" t="s">
         <v>94</v>
       </c>
@@ -7188,8 +8294,8 @@
         <v>1.4980736205850707</v>
       </c>
     </row>
-    <row r="83" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H84" s="20" t="s">
         <v>78</v>
       </c>
@@ -7209,7 +8315,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H85" s="23" t="s">
         <v>97</v>
       </c>
@@ -7232,7 +8338,7 @@
         <v>0.6675239362465053</v>
       </c>
     </row>
-    <row r="86" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H86" s="29" t="s">
         <v>100</v>
       </c>
@@ -7255,7 +8361,7 @@
         <v>0.3324760637534947</v>
       </c>
     </row>
-    <row r="87" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H87" s="29" t="s">
         <v>103</v>
       </c>
@@ -7278,7 +8384,7 @@
         <v>0.16653967382950344</v>
       </c>
     </row>
-    <row r="88" spans="2:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H88" s="23" t="s">
         <v>106</v>
       </c>
@@ -7301,8 +8407,8 @@
         <v>0.25110963243192053</v>
       </c>
     </row>
-    <row r="89" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="90" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="90" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H90" s="20" t="s">
         <v>78</v>
       </c>
@@ -7322,7 +8428,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H91" s="29" t="s">
         <v>109</v>
       </c>
@@ -7345,7 +8451,7 @@
         <v>2.3670627855666742E-2</v>
       </c>
     </row>
-    <row r="92" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H92" s="27" t="s">
         <v>112</v>
       </c>
@@ -7368,7 +8474,7 @@
         <v>0.70727024049996834</v>
       </c>
     </row>
-    <row r="93" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H93" s="23" t="s">
         <v>115</v>
       </c>
@@ -7391,8 +8497,8 @@
         <v>1.3353089361362267</v>
       </c>
     </row>
-    <row r="94" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="95" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B95" s="1" t="s">
         <v>0</v>
       </c>
@@ -7409,16 +8515,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="96" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="55" t="s">
+    <row r="96" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B96" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="56"/>
-      <c r="D96" s="56"/>
-      <c r="E96" s="56"/>
+      <c r="C96" s="50"/>
+      <c r="D96" s="50"/>
+      <c r="E96" s="50"/>
       <c r="F96" s="9"/>
     </row>
-    <row r="97" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B97" s="3" t="s">
         <v>119</v>
       </c>
@@ -7435,16 +8541,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="51" t="s">
+    <row r="98" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B98" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
-      <c r="E98" s="52"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
       <c r="F98" s="9"/>
     </row>
-    <row r="99" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B99" s="5" t="s">
         <v>121</v>
       </c>
@@ -7461,7 +8567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="100" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B100" s="5" t="s">
         <v>122</v>
       </c>
@@ -7478,7 +8584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="101" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B101" s="5" t="s">
         <v>123</v>
       </c>
@@ -7495,7 +8601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B102" s="5" t="s">
         <v>124</v>
       </c>
@@ -7512,7 +8618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B103" s="3" t="s">
         <v>125</v>
       </c>
@@ -7527,16 +8633,16 @@
       </c>
       <c r="F103" s="35"/>
     </row>
-    <row r="104" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="51" t="s">
+    <row r="104" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C104" s="52"/>
-      <c r="D104" s="52"/>
-      <c r="E104" s="52"/>
+      <c r="C104" s="57"/>
+      <c r="D104" s="57"/>
+      <c r="E104" s="57"/>
       <c r="F104" s="9"/>
     </row>
-    <row r="105" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B105" s="5" t="s">
         <v>126</v>
       </c>
@@ -7553,7 +8659,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B106" s="5" t="s">
         <v>127</v>
       </c>
@@ -7570,7 +8676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B107" s="5" t="s">
         <v>128</v>
       </c>
@@ -7587,7 +8693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="108" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B108" s="5" t="s">
         <v>129</v>
       </c>
@@ -7604,7 +8710,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B109" s="5" t="s">
         <v>130</v>
       </c>
@@ -7621,7 +8727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B110" s="3" t="s">
         <v>131</v>
       </c>
@@ -7638,16 +8744,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="111" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="55" t="s">
+    <row r="111" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C111" s="56"/>
-      <c r="D111" s="56"/>
-      <c r="E111" s="56"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="50"/>
       <c r="F111" s="9"/>
     </row>
-    <row r="112" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B112" s="3" t="s">
         <v>119</v>
       </c>
@@ -7664,16 +8770,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="113" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B113" s="51" t="s">
+    <row r="113" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C113" s="52"/>
-      <c r="D113" s="52"/>
-      <c r="E113" s="52"/>
+      <c r="C113" s="57"/>
+      <c r="D113" s="57"/>
+      <c r="E113" s="57"/>
       <c r="F113" s="9"/>
     </row>
-    <row r="114" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B114" s="5" t="s">
         <v>133</v>
       </c>
@@ -7690,7 +8796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B115" s="5" t="s">
         <v>134</v>
       </c>
@@ -7707,7 +8813,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B116" s="5" t="s">
         <v>135</v>
       </c>
@@ -7724,7 +8830,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B117" s="5" t="s">
         <v>136</v>
       </c>
@@ -7741,7 +8847,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B118" s="5" t="s">
         <v>124</v>
       </c>
@@ -7758,7 +8864,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B119" s="3" t="s">
         <v>125</v>
       </c>
@@ -7775,16 +8881,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B120" s="51" t="s">
+    <row r="120" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B120" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C120" s="52"/>
-      <c r="D120" s="52"/>
-      <c r="E120" s="52"/>
+      <c r="C120" s="57"/>
+      <c r="D120" s="57"/>
+      <c r="E120" s="57"/>
       <c r="F120" s="9"/>
     </row>
-    <row r="121" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B121" s="5" t="s">
         <v>137</v>
       </c>
@@ -7801,31 +8907,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B122" s="53" t="s">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B122" s="62" t="s">
         <v>153</v>
       </c>
-      <c r="C122" s="53">
+      <c r="C122" s="62">
         <v>4222</v>
       </c>
-      <c r="D122" s="57" t="s">
+      <c r="D122" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="E122" s="57" t="s">
+      <c r="E122" s="64" t="s">
         <v>154</v>
       </c>
-      <c r="F122" s="47" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B123" s="54"/>
-      <c r="C123" s="54"/>
-      <c r="D123" s="58"/>
-      <c r="E123" s="58"/>
-      <c r="F123" s="48"/>
-    </row>
-    <row r="124" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F122" s="58" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B123" s="63"/>
+      <c r="C123" s="63"/>
+      <c r="D123" s="65"/>
+      <c r="E123" s="65"/>
+      <c r="F123" s="59"/>
+    </row>
+    <row r="124" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B124" s="5" t="s">
         <v>138</v>
       </c>
@@ -7842,7 +8948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B125" s="5" t="s">
         <v>139</v>
       </c>
@@ -7859,7 +8965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B126" s="5" t="s">
         <v>140</v>
       </c>
@@ -7876,7 +8982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B127" s="3" t="s">
         <v>141</v>
       </c>
@@ -7893,7 +8999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B128" s="8" t="s">
         <v>0</v>
       </c>
@@ -7910,18 +9016,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B129" s="49" t="s">
+    <row r="129" spans="2:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B129" s="60" t="s">
         <v>142</v>
       </c>
-      <c r="C129" s="50"/>
-      <c r="D129" s="50"/>
+      <c r="C129" s="61"/>
+      <c r="D129" s="61"/>
       <c r="E129" s="31" t="s">
         <v>3</v>
       </c>
       <c r="F129" s="9"/>
     </row>
-    <row r="130" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B130" s="3" t="s">
         <v>119</v>
       </c>
@@ -7938,16 +9044,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="131" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B131" s="51" t="s">
+    <row r="131" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B131" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C131" s="52"/>
-      <c r="D131" s="52"/>
+      <c r="C131" s="57"/>
+      <c r="D131" s="57"/>
       <c r="E131" s="32"/>
       <c r="F131" s="9"/>
     </row>
-    <row r="132" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B132" s="5" t="s">
         <v>143</v>
       </c>
@@ -7964,7 +9070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="133" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B133" s="5" t="s">
         <v>144</v>
       </c>
@@ -7981,7 +9087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="134" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B134" s="5" t="s">
         <v>145</v>
       </c>
@@ -7998,7 +9104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="135" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B135" s="5" t="s">
         <v>146</v>
       </c>
@@ -8015,7 +9121,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B136" s="5" t="s">
         <v>147</v>
       </c>
@@ -8032,7 +9138,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B137" s="3" t="s">
         <v>125</v>
       </c>
@@ -8049,16 +9155,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B138" s="51" t="s">
+    <row r="138" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B138" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C138" s="52"/>
-      <c r="D138" s="52"/>
+      <c r="C138" s="57"/>
+      <c r="D138" s="57"/>
       <c r="E138" s="32"/>
       <c r="F138" s="9"/>
     </row>
-    <row r="139" spans="2:6" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B139" s="5" t="s">
         <v>148</v>
       </c>
@@ -8075,7 +9181,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="140" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B140" s="5" t="s">
         <v>149</v>
       </c>
@@ -8092,7 +9198,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="141" spans="2:6" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B141" s="5" t="s">
         <v>150</v>
       </c>
@@ -8109,7 +9215,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B142" s="5" t="s">
         <v>140</v>
       </c>
@@ -8126,7 +9232,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B143" s="3" t="s">
         <v>151</v>
       </c>
@@ -8143,7 +9249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B144" s="3" t="s">
         <v>152</v>
       </c>
@@ -8160,8 +9266,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="146" spans="2:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="146" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B146" s="39" t="s">
         <v>155</v>
       </c>
@@ -8178,7 +9284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B147" s="27" t="s">
         <v>157</v>
       </c>
@@ -8195,7 +9301,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B148" s="27" t="s">
         <v>158</v>
       </c>
@@ -8212,7 +9318,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="149" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B149" s="40" t="s">
         <v>159</v>
       </c>
@@ -8229,7 +9335,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B150" s="27" t="s">
         <v>160</v>
       </c>
@@ -8246,7 +9352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="151" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B151" s="27" t="s">
         <v>161</v>
       </c>
@@ -8263,7 +9369,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B152" s="40" t="s">
         <v>162</v>
       </c>
@@ -8280,7 +9386,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="153" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B153" s="27" t="s">
         <v>163</v>
       </c>
@@ -8297,7 +9403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="154" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B154" s="27" t="s">
         <v>164</v>
       </c>
@@ -8314,7 +9420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="155" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B155" s="27" t="s">
         <v>165</v>
       </c>
@@ -8331,7 +9437,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B156" s="27" t="s">
         <v>166</v>
       </c>
@@ -8348,7 +9454,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="157" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B157" s="27" t="s">
         <v>167</v>
       </c>
@@ -8365,7 +9471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B158" s="40" t="s">
         <v>168</v>
       </c>
@@ -8382,7 +9488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="159" spans="2:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B159" s="27" t="s">
         <v>169</v>
       </c>
@@ -8399,7 +9505,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B160" s="27" t="s">
         <v>170</v>
       </c>
@@ -8416,7 +9522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="161" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B161" s="27" t="s">
         <v>171</v>
       </c>
@@ -8433,7 +9539,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B162" s="27" t="s">
         <v>172</v>
       </c>
@@ -8450,7 +9556,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B163" s="27" t="s">
         <v>173</v>
       </c>
@@ -8467,7 +9573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="164" spans="2:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B164" s="40" t="s">
         <v>174</v>
       </c>
@@ -8484,8 +9590,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="165" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="166" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="166" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H166" s="20" t="s">
         <v>78</v>
       </c>
@@ -8505,7 +9611,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H167" s="23" t="s">
         <v>175</v>
       </c>
@@ -8532,7 +9638,7 @@
         <v>81183</v>
       </c>
     </row>
-    <row r="168" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H168" s="23" t="s">
         <v>177</v>
       </c>
@@ -8552,7 +9658,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H169" s="29" t="s">
         <v>179</v>
       </c>
@@ -8572,7 +9678,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H170" s="23" t="s">
         <v>181</v>
       </c>
@@ -8592,7 +9698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="171" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H171" s="23" t="s">
         <v>182</v>
       </c>
@@ -8612,7 +9718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="172" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H172" s="27" t="s">
         <v>183</v>
       </c>
@@ -8632,7 +9738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H173" s="27" t="s">
         <v>185</v>
       </c>
@@ -8652,7 +9758,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H174" s="27" t="s">
         <v>187</v>
       </c>
@@ -8672,7 +9778,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="175" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H175" s="27" t="s">
         <v>188</v>
       </c>
@@ -8692,7 +9798,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="176" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:16" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H176" s="27" t="s">
         <v>189</v>
       </c>
@@ -8712,8 +9818,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="177" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="178" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="8:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="178" spans="8:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H178" s="20" t="s">
         <v>78</v>
       </c>
@@ -8733,7 +9839,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="8:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H179" s="23" t="s">
         <v>192</v>
       </c>
@@ -8753,7 +9859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="180" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="8:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H180" s="27" t="s">
         <v>194</v>
       </c>
@@ -8773,7 +9879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="181" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H181" s="29" t="s">
         <v>196</v>
       </c>
@@ -8795,7 +9901,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="182" spans="8:13" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H182" s="29" t="s">
         <v>198</v>
       </c>
@@ -8817,7 +9923,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="183" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H183" s="23" t="s">
         <v>199</v>
       </c>
@@ -8839,7 +9945,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="184" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H184" s="23" t="s">
         <v>202</v>
       </c>
@@ -8861,7 +9967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="185" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H185" s="23" t="s">
         <v>205</v>
       </c>
@@ -8883,7 +9989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="8:13" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="8:13" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H186" s="23" t="s">
         <v>217</v>
       </c>
@@ -8905,7 +10011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="187" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="8:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H187" s="23" t="s">
         <v>218</v>
       </c>
@@ -8927,7 +10033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="188" spans="8:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="8:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H188" s="23" t="s">
         <v>219</v>
       </c>
@@ -8949,21 +10055,1035 @@
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="189" spans="8:13" x14ac:dyDescent="0.3">
       <c r="I189" s="45"/>
     </row>
+    <row r="205" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="206" spans="2:6" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B206" s="39" t="s">
+        <v>227</v>
+      </c>
+      <c r="C206" s="21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D206" s="21">
+        <v>1</v>
+      </c>
+      <c r="E206" s="21">
+        <v>2</v>
+      </c>
+      <c r="F206" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B207" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="C207" s="25">
+        <v>5610</v>
+      </c>
+      <c r="D207" s="41">
+        <v>209476</v>
+      </c>
+      <c r="E207" s="41">
+        <v>159523</v>
+      </c>
+      <c r="F207" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="2:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B208" s="48" t="s">
+        <v>222</v>
+      </c>
+      <c r="C208" s="25">
+        <v>5620</v>
+      </c>
+      <c r="D208" s="41">
+        <v>712203</v>
+      </c>
+      <c r="E208" s="41">
+        <v>503558</v>
+      </c>
+      <c r="F208" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B209" s="48" t="s">
+        <v>223</v>
+      </c>
+      <c r="C209" s="25">
+        <v>5630</v>
+      </c>
+      <c r="D209" s="41">
+        <v>206547</v>
+      </c>
+      <c r="E209" s="41">
+        <v>175200</v>
+      </c>
+      <c r="F209" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B210" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="C210" s="25">
+        <v>5640</v>
+      </c>
+      <c r="D210" s="41">
+        <v>129085</v>
+      </c>
+      <c r="E210" s="41">
+        <v>94678</v>
+      </c>
+      <c r="F210" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B211" s="48" t="s">
+        <v>225</v>
+      </c>
+      <c r="C211" s="25">
+        <v>5650</v>
+      </c>
+      <c r="D211" s="41">
+        <v>141899</v>
+      </c>
+      <c r="E211" s="41">
+        <v>203564</v>
+      </c>
+      <c r="F211" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B212" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="C212" s="25">
+        <v>5660</v>
+      </c>
+      <c r="D212" s="41">
+        <v>1399210</v>
+      </c>
+      <c r="E212" s="41">
+        <v>1136523</v>
+      </c>
+      <c r="F212" s="41" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="213" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D213" s="15"/>
+    </row>
+    <row r="214" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D214" s="15"/>
+      <c r="H214" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="I214" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="J214" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K214" s="21">
+        <v>1</v>
+      </c>
+      <c r="L214" s="21">
+        <v>2</v>
+      </c>
+      <c r="M214" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="215" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E215" s="15"/>
+      <c r="F215" s="15"/>
+      <c r="H215" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="I215" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="J215" s="25">
+        <v>5610</v>
+      </c>
+      <c r="K215" s="41">
+        <f>D207</f>
+        <v>209476</v>
+      </c>
+      <c r="L215" s="41">
+        <f>E207</f>
+        <v>159523</v>
+      </c>
+      <c r="M215" s="41"/>
+    </row>
+    <row r="216" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H216" s="47" t="s">
+        <v>233</v>
+      </c>
+      <c r="I216" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J216" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="K216" s="41">
+        <f>D208+D209</f>
+        <v>918750</v>
+      </c>
+      <c r="L216" s="41">
+        <f>E208+E209</f>
+        <v>678758</v>
+      </c>
+      <c r="M216" s="41"/>
+    </row>
+    <row r="217" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H217" s="47" t="s">
+        <v>236</v>
+      </c>
+      <c r="I217" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="J217" s="25">
+        <v>5640</v>
+      </c>
+      <c r="K217" s="41">
+        <f>D210</f>
+        <v>129085</v>
+      </c>
+      <c r="L217" s="41">
+        <f>E210</f>
+        <v>94678</v>
+      </c>
+      <c r="M217" s="41"/>
+    </row>
+    <row r="218" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H218" s="47" t="s">
+        <v>238</v>
+      </c>
+      <c r="I218" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J218" s="25">
+        <v>5650</v>
+      </c>
+      <c r="K218" s="41">
+        <f>D211</f>
+        <v>141899</v>
+      </c>
+      <c r="L218" s="41">
+        <f>E211</f>
+        <v>203564</v>
+      </c>
+      <c r="M218" s="41"/>
+    </row>
+    <row r="219" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H219" s="47" t="s">
+        <v>240</v>
+      </c>
+      <c r="I219" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="J219" s="25">
+        <v>5660</v>
+      </c>
+      <c r="K219" s="41">
+        <f>D212</f>
+        <v>1399210</v>
+      </c>
+      <c r="L219" s="41">
+        <f>E212</f>
+        <v>1136523</v>
+      </c>
+      <c r="M219" s="41"/>
+    </row>
+    <row r="220" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H220" s="47" t="s">
+        <v>242</v>
+      </c>
+      <c r="I220" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="J220" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="K220" s="70">
+        <f>K215/K$219</f>
+        <v>0.14971019360925095</v>
+      </c>
+      <c r="L220" s="70">
+        <f>L215/L$219</f>
+        <v>0.1403605558356496</v>
+      </c>
+      <c r="M220" s="70"/>
+    </row>
+    <row r="221" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H221" s="47" t="s">
+        <v>244</v>
+      </c>
+      <c r="I221" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="J221" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="K221" s="70">
+        <f t="shared" ref="K221:L223" si="12">K216/K$219</f>
+        <v>0.65662052158003448</v>
+      </c>
+      <c r="L221" s="70">
+        <f t="shared" si="12"/>
+        <v>0.59722328540645464</v>
+      </c>
+      <c r="M221" s="70"/>
+    </row>
+    <row r="222" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H222" s="47" t="s">
+        <v>246</v>
+      </c>
+      <c r="I222" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="J222" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="K222" s="70">
+        <f t="shared" si="12"/>
+        <v>9.2255629962621766E-2</v>
+      </c>
+      <c r="L222" s="70">
+        <f t="shared" si="12"/>
+        <v>8.3304957312786448E-2</v>
+      </c>
+      <c r="M222" s="70"/>
+    </row>
+    <row r="223" spans="2:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H223" s="47" t="s">
+        <v>248</v>
+      </c>
+      <c r="I223" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="J223" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="K223" s="70">
+        <f t="shared" si="12"/>
+        <v>0.10141365484809285</v>
+      </c>
+      <c r="L223" s="70">
+        <f t="shared" si="12"/>
+        <v>0.17911120144510934</v>
+      </c>
+      <c r="M223" s="70"/>
+    </row>
+    <row r="224" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K224" s="71"/>
+      <c r="L224" s="71"/>
+    </row>
+    <row r="225" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H225" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="I225" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="J225" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="K225" s="21">
+        <v>1</v>
+      </c>
+      <c r="L225" s="21">
+        <v>2</v>
+      </c>
+      <c r="M225" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H226" s="47" t="s">
+        <v>250</v>
+      </c>
+      <c r="I226" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="J226" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="K226" s="30">
+        <f>K215/K$167</f>
+        <v>0.14150026378130673</v>
+      </c>
+      <c r="L226" s="30">
+        <f>L215/L$167</f>
+        <v>0.12868047718650655</v>
+      </c>
+      <c r="M226" s="69"/>
+    </row>
+    <row r="227" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H227" s="47" t="s">
+        <v>253</v>
+      </c>
+      <c r="I227" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="J227" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="K227" s="30">
+        <f t="shared" ref="K227:L230" si="13">K216/K$167</f>
+        <v>0.62061222932018723</v>
+      </c>
+      <c r="L227" s="30">
+        <f t="shared" si="13"/>
+        <v>0.54752545610450409</v>
+      </c>
+      <c r="M227" s="69"/>
+    </row>
+    <row r="228" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H228" s="47" t="s">
+        <v>256</v>
+      </c>
+      <c r="I228" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="J228" s="24" t="s">
+        <v>258</v>
+      </c>
+      <c r="K228" s="30">
+        <f t="shared" si="13"/>
+        <v>8.719644040467632E-2</v>
+      </c>
+      <c r="L228" s="30">
+        <f t="shared" si="13"/>
+        <v>7.637275013047691E-2</v>
+      </c>
+      <c r="M228" s="69"/>
+    </row>
+    <row r="229" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H229" s="47" t="s">
+        <v>259</v>
+      </c>
+      <c r="I229" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="J229" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="K229" s="30">
+        <f t="shared" si="13"/>
+        <v>9.5852250044413875E-2</v>
+      </c>
+      <c r="L229" s="30">
+        <f t="shared" si="13"/>
+        <v>0.16420649472486112</v>
+      </c>
+      <c r="M229" s="69"/>
+    </row>
+    <row r="230" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H230" s="47" t="s">
+        <v>262</v>
+      </c>
+      <c r="I230" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="J230" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="K230" s="30">
+        <f>K219/K$167</f>
+        <v>0.94516118355058421</v>
+      </c>
+      <c r="L230" s="30">
+        <f t="shared" si="13"/>
+        <v>0.91678517814634874</v>
+      </c>
+      <c r="M230" s="69"/>
+    </row>
+    <row r="231" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="232" spans="1:13" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A232" s="39" t="s">
+        <v>228</v>
+      </c>
+      <c r="B232" s="21" t="s">
+        <v>229</v>
+      </c>
+      <c r="C232" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="D232" s="21">
+        <v>1</v>
+      </c>
+      <c r="E232" s="21">
+        <v>2</v>
+      </c>
+      <c r="F232" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A233" s="47" t="s">
+        <v>265</v>
+      </c>
+      <c r="B233" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C233" s="25">
+        <v>2210</v>
+      </c>
+      <c r="D233" s="14">
+        <v>0</v>
+      </c>
+      <c r="E233" s="14">
+        <v>0</v>
+      </c>
+      <c r="F233" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A234" s="47" t="s">
+        <v>267</v>
+      </c>
+      <c r="B234" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="C234" s="25">
+        <v>2220</v>
+      </c>
+      <c r="D234" s="14">
+        <v>153445</v>
+      </c>
+      <c r="E234" s="14">
+        <v>128457</v>
+      </c>
+      <c r="F234" s="69" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="236" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J236" s="39" t="s">
+        <v>269</v>
+      </c>
+      <c r="K236" s="21">
+        <v>1</v>
+      </c>
+      <c r="L236" s="21">
+        <v>2</v>
+      </c>
+      <c r="M236" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J237" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="K237" s="28">
+        <f>K215+K216+K217+K218</f>
+        <v>1399210</v>
+      </c>
+      <c r="L237" s="28">
+        <f>L215+L216+L217+L218</f>
+        <v>1136523</v>
+      </c>
+      <c r="M237" s="25"/>
+    </row>
+    <row r="238" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J238" s="72" t="s">
+        <v>271</v>
+      </c>
+      <c r="K238" s="28">
+        <f>K237+D233-D234</f>
+        <v>1245765</v>
+      </c>
+      <c r="L238" s="28">
+        <f>L237+E233-E234</f>
+        <v>1008066</v>
+      </c>
+      <c r="M238" s="25"/>
+    </row>
+    <row r="239" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J239" s="72" t="s">
+        <v>272</v>
+      </c>
+      <c r="K239" s="28">
+        <f>1.357*K238</f>
+        <v>1690503.105</v>
+      </c>
+      <c r="L239" s="28">
+        <f>1.357*L238</f>
+        <v>1367945.5619999999</v>
+      </c>
+      <c r="M239" s="25"/>
+    </row>
+    <row r="240" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="241" spans="1:6" ht="45.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A241" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B241" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C241" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D241" s="21">
+        <v>1</v>
+      </c>
+      <c r="E241" s="21">
+        <v>2</v>
+      </c>
+      <c r="F241" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A242" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="B242" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C242" s="25">
+        <v>2110</v>
+      </c>
+      <c r="D242" s="41">
+        <f>D147</f>
+        <v>1480393</v>
+      </c>
+      <c r="E242" s="41">
+        <f>E147</f>
+        <v>1239683</v>
+      </c>
+      <c r="F242" s="67"/>
+    </row>
+    <row r="243" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A243" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="B243" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C243" s="25">
+        <v>1210</v>
+      </c>
+      <c r="D243" s="41">
+        <f>D14</f>
+        <v>38279</v>
+      </c>
+      <c r="E243" s="41">
+        <f>E14</f>
+        <v>35789</v>
+      </c>
+      <c r="F243" s="67"/>
+    </row>
+    <row r="244" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A244" s="47" t="s">
+        <v>275</v>
+      </c>
+      <c r="B244" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="C244" s="25">
+        <v>1200</v>
+      </c>
+      <c r="D244" s="41">
+        <f>D19</f>
+        <v>408946</v>
+      </c>
+      <c r="E244" s="41">
+        <f>E19</f>
+        <v>498978</v>
+      </c>
+      <c r="F244" s="67"/>
+    </row>
+    <row r="245" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A245" s="47" t="s">
+        <v>277</v>
+      </c>
+      <c r="B245" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="C245" s="25">
+        <v>1600</v>
+      </c>
+      <c r="D245" s="41">
+        <f>D20</f>
+        <v>1103010</v>
+      </c>
+      <c r="E245" s="41">
+        <f>E20</f>
+        <v>1029180</v>
+      </c>
+      <c r="F245" s="67"/>
+    </row>
+    <row r="246" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A246" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="B246" s="24" t="s">
+        <v>280</v>
+      </c>
+      <c r="C246" s="25" t="s">
+        <v>281</v>
+      </c>
+      <c r="D246" s="67">
+        <f>D242/D245</f>
+        <v>1.3421392371782668</v>
+      </c>
+      <c r="E246" s="67">
+        <f>E242/E245</f>
+        <v>1.2045346780932393</v>
+      </c>
+      <c r="F246" s="67"/>
+    </row>
+    <row r="247" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="B247" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="C247" s="25" t="s">
+        <v>284</v>
+      </c>
+      <c r="D247" s="67">
+        <f>D242/D244</f>
+        <v>3.6200207362341237</v>
+      </c>
+      <c r="E247" s="67">
+        <f>E242/E244</f>
+        <v>2.4844442039528798</v>
+      </c>
+      <c r="F247" s="67"/>
+    </row>
+    <row r="248" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A248" s="73" t="s">
+        <v>285</v>
+      </c>
+      <c r="B248" s="53" t="s">
+        <v>286</v>
+      </c>
+      <c r="C248" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="D248" s="74">
+        <f>D242/D243</f>
+        <v>38.673763682436842</v>
+      </c>
+      <c r="E248" s="74">
+        <f>E242/E243</f>
+        <v>34.638659923440166</v>
+      </c>
+      <c r="F248" s="74"/>
+    </row>
+    <row r="249" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A249" s="47" t="s">
+        <v>273</v>
+      </c>
+      <c r="B249" s="54"/>
+      <c r="C249" s="54"/>
+      <c r="D249" s="75"/>
+      <c r="E249" s="75"/>
+      <c r="F249" s="75"/>
+    </row>
+    <row r="250" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="251" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A251" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="B251" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C251" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D251" s="21">
+        <v>1</v>
+      </c>
+      <c r="E251" s="21">
+        <v>2</v>
+      </c>
+      <c r="F251" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A252" s="47" t="s">
+        <v>288</v>
+      </c>
+      <c r="B252" s="24" t="s">
+        <v>289</v>
+      </c>
+      <c r="C252" s="25">
+        <v>1230</v>
+      </c>
+      <c r="D252" s="78">
+        <f>D16</f>
+        <v>244446</v>
+      </c>
+      <c r="E252" s="78">
+        <f>E16</f>
+        <v>195844</v>
+      </c>
+      <c r="F252" s="77"/>
+    </row>
+    <row r="253" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A253" s="48" t="s">
+        <v>290</v>
+      </c>
+      <c r="B253" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="C253" s="25">
+        <v>1520</v>
+      </c>
+      <c r="D253" s="78">
+        <f>D37</f>
+        <v>152401</v>
+      </c>
+      <c r="E253" s="78">
+        <f>E37</f>
+        <v>184298</v>
+      </c>
+      <c r="F253" s="77"/>
+    </row>
+    <row r="254" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A254" s="47" t="s">
+        <v>292</v>
+      </c>
+      <c r="B254" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="C254" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="D254" s="78">
+        <v>360</v>
+      </c>
+      <c r="E254" s="78">
+        <v>360</v>
+      </c>
+      <c r="F254" s="77"/>
+    </row>
+    <row r="255" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A255" s="48" t="s">
+        <v>295</v>
+      </c>
+      <c r="B255" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="C255" s="25" t="s">
+        <v>297</v>
+      </c>
+      <c r="D255" s="77">
+        <f>360/D248</f>
+        <v>9.3086362877965527</v>
+      </c>
+      <c r="E255" s="77">
+        <f>360/E248</f>
+        <v>10.393011761877833</v>
+      </c>
+      <c r="F255" s="77"/>
+    </row>
+    <row r="256" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A256" s="48" t="s">
+        <v>298</v>
+      </c>
+      <c r="B256" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="C256" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="D256" s="77">
+        <f>360*D252/D242</f>
+        <v>59.444053031863838</v>
+      </c>
+      <c r="E256" s="77">
+        <f>360*E252/E242</f>
+        <v>56.872474656827592</v>
+      </c>
+      <c r="F256" s="77"/>
+    </row>
+    <row r="257" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A257" s="76" t="s">
+        <v>301</v>
+      </c>
+      <c r="B257" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="C257" s="25" t="s">
+        <v>303</v>
+      </c>
+      <c r="D257" s="77">
+        <f>360*D253/D242</f>
+        <v>37.060672402530948</v>
+      </c>
+      <c r="E257" s="77">
+        <f>360*E253/E242</f>
+        <v>53.519552982496329</v>
+      </c>
+      <c r="F257" s="77"/>
+    </row>
+    <row r="258" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A258" s="47" t="s">
+        <v>304</v>
+      </c>
+      <c r="B258" s="24" t="s">
+        <v>305</v>
+      </c>
+      <c r="C258" s="25" t="s">
+        <v>306</v>
+      </c>
+      <c r="D258" s="77">
+        <f>D255+D256</f>
+        <v>68.752689319660391</v>
+      </c>
+      <c r="E258" s="77">
+        <f>E255+E256</f>
+        <v>67.265486418705422</v>
+      </c>
+      <c r="F258" s="77"/>
+    </row>
+    <row r="259" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A259" s="48" t="s">
+        <v>307</v>
+      </c>
+      <c r="B259" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="C259" s="25" t="s">
+        <v>309</v>
+      </c>
+      <c r="D259" s="77">
+        <f>D258-D257</f>
+        <v>31.692016917129443</v>
+      </c>
+      <c r="E259" s="77">
+        <f>E258-E257</f>
+        <v>13.745933436209093</v>
+      </c>
+      <c r="F259" s="77"/>
+    </row>
+    <row r="260" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="261" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A261" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B261" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C261" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="D261" s="21">
+        <v>1</v>
+      </c>
+      <c r="E261" s="21">
+        <v>2</v>
+      </c>
+      <c r="F261" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A262" s="80" t="s">
+        <v>310</v>
+      </c>
+      <c r="B262" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="C262" s="81" t="s">
+        <v>312</v>
+      </c>
+      <c r="D262" s="68">
+        <f>K180/D242</f>
+        <v>3.2030008247809875E-2</v>
+      </c>
+      <c r="E262" s="68">
+        <f>L180/E242</f>
+        <v>3.8249294376062268E-2</v>
+      </c>
+      <c r="F262" s="68"/>
+    </row>
+    <row r="263" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A263" s="80" t="s">
+        <v>313</v>
+      </c>
+      <c r="B263" s="24" t="s">
+        <v>314</v>
+      </c>
+      <c r="C263" s="81" t="s">
+        <v>315</v>
+      </c>
+      <c r="D263" s="68">
+        <f>K180/K47</f>
+        <v>4.2988730836529133E-2</v>
+      </c>
+      <c r="E263" s="68">
+        <f>L180/L47</f>
+        <v>4.6072601488563708E-2</v>
+      </c>
+      <c r="F263" s="68"/>
+    </row>
+    <row r="264" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A264" s="80" t="s">
+        <v>316</v>
+      </c>
+      <c r="B264" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="C264" s="82" t="s">
+        <v>318</v>
+      </c>
+      <c r="D264" s="68">
+        <f>K180/K53</f>
+        <v>6.048318175440387E-2</v>
+      </c>
+      <c r="E264" s="68">
+        <f>L180/L53</f>
+        <v>6.4376988997382395E-2</v>
+      </c>
+      <c r="F264" s="68"/>
+    </row>
+    <row r="265" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A265" s="83" t="s">
+        <v>319</v>
+      </c>
+      <c r="B265" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="C265" s="81" t="s">
+        <v>321</v>
+      </c>
+      <c r="D265" s="68">
+        <f>K180/(K53+K54)</f>
+        <v>6.047855311658993E-2</v>
+      </c>
+      <c r="E265" s="68">
+        <f>L180/(L53+L54)</f>
+        <v>6.4339427557253775E-2</v>
+      </c>
+      <c r="F265" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B96:E96"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="I78:I79"/>
-    <mergeCell ref="K78:K79"/>
-    <mergeCell ref="L78:L79"/>
-    <mergeCell ref="M78:M79"/>
-    <mergeCell ref="B98:E98"/>
-    <mergeCell ref="B104:E104"/>
-    <mergeCell ref="B111:E111"/>
-    <mergeCell ref="B113:E113"/>
+  <mergeCells count="24">
+    <mergeCell ref="B248:B249"/>
+    <mergeCell ref="C248:C249"/>
+    <mergeCell ref="D248:D249"/>
+    <mergeCell ref="E248:E249"/>
+    <mergeCell ref="F248:F249"/>
     <mergeCell ref="B120:E120"/>
     <mergeCell ref="F122:F123"/>
     <mergeCell ref="B129:D129"/>
@@ -8973,8 +11093,19 @@
     <mergeCell ref="C122:C123"/>
     <mergeCell ref="D122:D123"/>
     <mergeCell ref="E122:E123"/>
+    <mergeCell ref="M78:M79"/>
+    <mergeCell ref="B98:E98"/>
+    <mergeCell ref="B104:E104"/>
+    <mergeCell ref="B111:E111"/>
+    <mergeCell ref="B113:E113"/>
+    <mergeCell ref="B96:E96"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="K78:K79"/>
+    <mergeCell ref="L78:L79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>